<commit_message>
Corrected parts list - one of the 0.01 uF capacitors is 0402 size
</commit_message>
<xml_diff>
--- a/parts_list.xlsx
+++ b/parts_list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
   <si>
     <t>Omnetics connector</t>
   </si>
@@ -153,15 +153,9 @@
     <t>http://www.digikey.com/product-search/en?FV=fff40002%2Cfff8000b%2C1c0002%2C3400b0%2C380004%2C400004&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=1000011&amp;page=1&amp;stock=1&amp;pbfree=0&amp;rohs=0&amp;quantity=&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
   </si>
   <si>
-    <t>http://www.digikey.com/short/tnjpd2</t>
-  </si>
-  <si>
     <t>cart for 10</t>
   </si>
   <si>
-    <t>http://www.digikey.com/short/tnjzq5</t>
-  </si>
-  <si>
     <t>cart for 1</t>
   </si>
   <si>
@@ -169,6 +163,21 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Capacitor (0.1 uF, 25V, 0402 package)</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/GRM155R71E103KA01D/490-1312-1-ND/587934</t>
+  </si>
+  <si>
+    <t>GRM155R71E103KA01D</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/short/tn2vf4</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/short/tn2vvz</t>
   </si>
 </sst>
 </file>
@@ -518,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,7 +542,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
@@ -548,16 +557,16 @@
         <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" t="s">
         <v>45</v>
       </c>
-      <c r="M1" t="s">
-        <v>46</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -568,7 +577,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -676,7 +685,7 @@
         <v>30</v>
       </c>
       <c r="E8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>26</v>
@@ -684,64 +693,82 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
         <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
         <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G12" t="s">
         <v>41</v>
       </c>
     </row>
@@ -749,9 +776,9 @@
   <hyperlinks>
     <hyperlink ref="D7" r:id="rId1"/>
     <hyperlink ref="D8" r:id="rId2"/>
-    <hyperlink ref="D9" r:id="rId3"/>
-    <hyperlink ref="D10" r:id="rId4"/>
-    <hyperlink ref="D11" r:id="rId5"/>
+    <hyperlink ref="D10" r:id="rId3"/>
+    <hyperlink ref="D11" r:id="rId4"/>
+    <hyperlink ref="D12" r:id="rId5"/>
     <hyperlink ref="H1" r:id="rId6"/>
     <hyperlink ref="N1" r:id="rId7"/>
     <hyperlink ref="D6" r:id="rId8"/>

</xml_diff>

<commit_message>
Corrected capacitors in parts list
</commit_message>
<xml_diff>
--- a/parts_list.xlsx
+++ b/parts_list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
   <si>
     <t>Omnetics connector</t>
   </si>
@@ -102,15 +102,6 @@
     <t>Capacitor (0.1 uF, 25V, 0201 package)</t>
   </si>
   <si>
-    <t>Murata Electronics North America</t>
-  </si>
-  <si>
-    <t>GRM033R61E103KA12D</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-detail/en/GRM033R61E103KA12D/490-7194-1-ND/3900511</t>
-  </si>
-  <si>
     <t>Capacitor (10 uF, 25V, 0603 package)</t>
   </si>
   <si>
@@ -165,19 +156,31 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Capacitor (0.1 uF, 25V, 0402 package)</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-detail/en/GRM155R71E103KA01D/490-1312-1-ND/587934</t>
-  </si>
-  <si>
-    <t>GRM155R71E103KA01D</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/short/tn2vf4</t>
   </si>
   <si>
     <t>http://www.digikey.com/short/tn2vvz</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>Capacitor (0.01 uF, 25V, 0402 package)</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C1, C2, C4, C6</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/C0603X5R1E104K030BB/445-13671-1-ND/3955337</t>
   </si>
 </sst>
 </file>
@@ -527,264 +530,264 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="61" customWidth="1"/>
+    <col min="2" max="3" width="34" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>48</v>
       </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>52</v>
       </c>
-      <c r="M1" t="s">
-        <v>45</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2">
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8">
-        <v>4</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="G12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" t="s">
         <v>38</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D7" r:id="rId1"/>
-    <hyperlink ref="D8" r:id="rId2"/>
-    <hyperlink ref="D10" r:id="rId3"/>
-    <hyperlink ref="D11" r:id="rId4"/>
-    <hyperlink ref="D12" r:id="rId5"/>
-    <hyperlink ref="H1" r:id="rId6"/>
-    <hyperlink ref="N1" r:id="rId7"/>
-    <hyperlink ref="D6" r:id="rId8"/>
-    <hyperlink ref="D5" r:id="rId9"/>
-    <hyperlink ref="D4" r:id="rId10"/>
-    <hyperlink ref="D3" r:id="rId11"/>
+    <hyperlink ref="E7" r:id="rId1"/>
+    <hyperlink ref="E10" r:id="rId2"/>
+    <hyperlink ref="E11" r:id="rId3"/>
+    <hyperlink ref="E12" r:id="rId4"/>
+    <hyperlink ref="I1" r:id="rId5"/>
+    <hyperlink ref="O1" r:id="rId6"/>
+    <hyperlink ref="E6" r:id="rId7"/>
+    <hyperlink ref="E5" r:id="rId8"/>
+    <hyperlink ref="E4" r:id="rId9"/>
+    <hyperlink ref="E3" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Removed resistor to ground before blocking capacitors
</commit_message>
<xml_diff>
--- a/parts_list.xlsx
+++ b/parts_list.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26621"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="11740" yWindow="0" windowWidth="13800" windowHeight="21120"/>
+    <workbookView xWindow="11745" yWindow="0" windowWidth="13800" windowHeight="15870"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="91">
   <si>
     <t>Omnetics connector</t>
   </si>
@@ -72,12 +72,6 @@
   </si>
   <si>
     <t>R7-R11</t>
-  </si>
-  <si>
-    <t>R12-R16</t>
-  </si>
-  <si>
-    <t>Bias return for instrumentation amplifier inputs</t>
   </si>
   <si>
     <t>Gain setting resistor for instrumentation amplifier (gain=100)</t>
@@ -676,27 +670,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="3"/>
+    <col min="1" max="1" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="3"/>
     <col min="3" max="3" width="49" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="61" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="3"/>
+    <col min="8" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>3</v>
@@ -720,7 +714,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>6</v>
@@ -729,9 +723,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -740,7 +734,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>4</v>
@@ -749,254 +743,254 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="G3" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B8" s="3">
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B9" s="3">
         <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="G10" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B11" s="3">
         <v>4</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="3" t="s">
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
-      <c r="A12" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="B12" s="3">
         <v>2</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" s="3" t="s">
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="B13" s="3">
         <v>5</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>85</v>
-      </c>
       <c r="G13" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1007,19 +1001,19 @@
         <v>13</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="G14" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1027,22 +1021,22 @@
         <v>4</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -1050,30 +1044,19 @@
         <v>5</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D16" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="3">
-        <v>5</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1097,7 +1080,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1114,7 +1097,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Updated parts list - added I2C pull up resistors (R10-R11)
</commit_message>
<xml_diff>
--- a/parts_list.xlsx
+++ b/parts_list.xlsx
@@ -673,7 +673,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,7 +713,7 @@
       <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="1" t="s">
         <v>90</v>
       </c>
       <c r="O1" s="3" t="s">
@@ -1063,6 +1063,7 @@
   <hyperlinks>
     <hyperlink ref="P1" r:id="rId1"/>
     <hyperlink ref="G11" r:id="rId2"/>
+    <hyperlink ref="J1" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Updated parts list C4 changed to ceramic type (from tantalum) C13-C17 changed to 6800pF (from 47nF) R7-R11 changed to 10M (from 1.5M)
</commit_message>
<xml_diff>
--- a/parts_list.xlsx
+++ b/parts_list.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="92">
   <si>
     <t>Omnetics connector</t>
   </si>
@@ -170,18 +170,6 @@
     <t>0402, Ceramic, X7R, 0.1uF, 10%, 16V</t>
   </si>
   <si>
-    <t>10 uF, Tantalum</t>
-  </si>
-  <si>
-    <t>AVX Corporation</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/short/3tt1dv</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> TLCK106M006QTA </t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
@@ -191,9 +179,6 @@
     <t>Voltage regulator for digital electronics</t>
   </si>
   <si>
-    <t>2.5 V low dropout linear voltage regulator</t>
-  </si>
-  <si>
     <t>Texas Instruments</t>
   </si>
   <si>
@@ -269,31 +254,49 @@
     <t>High pass filter for electrodes and virtual ground (with R7-R11)</t>
   </si>
   <si>
-    <t>http://www.digikey.com/short/3t3hqn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRM033R61C473KE84D </t>
-  </si>
-  <si>
-    <t>0201, Ceramic, X5R, 47nF, 10%, 16V</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/short/3t3hjp</t>
   </si>
   <si>
-    <t>0201, 1.5MOhm, 1%, 1/20W</t>
-  </si>
-  <si>
     <t>Rohm Semiconductor</t>
   </si>
   <si>
-    <t xml:space="preserve">MCR006YRTF1504 </t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/short/3t3h4w</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/short/3t3hmf</t>
+  </si>
+  <si>
+    <t>0201, 10MOhm, 1%, 1/20W</t>
+  </si>
+  <si>
+    <t>MCR006YRTF1005</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/short/38853w</t>
+  </si>
+  <si>
+    <t>TDK Corporation</t>
+  </si>
+  <si>
+    <t>CGA1A2X7R1C682K030BA</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/short/38852m</t>
+  </si>
+  <si>
+    <t>0201, Ceramic, X7R, 6800pF, 10%, 16V</t>
+  </si>
+  <si>
+    <t>2.5 V linear voltage regulator</t>
+  </si>
+  <si>
+    <t>Samsung Electro-Mechanics America, Inc.</t>
+  </si>
+  <si>
+    <t>0502, Ceramic, X5R, 10uF, 20% 10V</t>
+  </si>
+  <si>
+    <t>CL05A106MP5NUNC</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/short/388517</t>
   </si>
 </sst>
 </file>
@@ -673,17 +676,17 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" style="3"/>
     <col min="3" max="3" width="49" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="61" style="3" customWidth="1"/>
     <col min="8" max="16384" width="8.85546875" style="3"/>
   </cols>
@@ -714,7 +717,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>6</v>
@@ -759,36 +762,36 @@
       <c r="F3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
@@ -863,16 +866,16 @@
         <v>36</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -883,111 +886,111 @@
         <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>42</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>42</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B11" s="3">
         <v>4</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>42</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B12" s="3">
         <v>2</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>42</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B13" s="3">
         <v>5</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>83</v>
-      </c>
       <c r="G13" s="3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -1010,7 +1013,7 @@
         <v>21</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -1044,19 +1047,19 @@
         <v>5</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="E16" s="3" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1064,6 +1067,7 @@
     <hyperlink ref="P1" r:id="rId1"/>
     <hyperlink ref="G11" r:id="rId2"/>
     <hyperlink ref="J1" r:id="rId3"/>
+    <hyperlink ref="G3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
formatted parts list for thesis
</commit_message>
<xml_diff>
--- a/parts_list.xlsx
+++ b/parts_list.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11209"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2113F0E-9C99-0F44-8541-470A21B7004E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11745" yWindow="0" windowWidth="13800" windowHeight="15870"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$F$16</definedName>
+  </definedNames>
   <calcPr calcId="122211" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -32,9 +36,6 @@
     <t>Part Number</t>
   </si>
   <si>
-    <t>Quantity</t>
-  </si>
-  <si>
     <t>Omnetics</t>
   </si>
   <si>
@@ -125,9 +126,6 @@
     <t>AD8224</t>
   </si>
   <si>
-    <t>Name on board</t>
-  </si>
-  <si>
     <t>C4</t>
   </si>
   <si>
@@ -297,13 +295,19 @@
   </si>
   <si>
     <t>http://www.digikey.com/short/388517</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Qty</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -327,21 +331,50 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -356,14 +389,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -381,6 +432,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -429,7 +483,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -462,9 +516,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -497,6 +568,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -672,405 +760,408 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="50" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="3"/>
-    <col min="3" max="3" width="49" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="3.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="20.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="26.5" style="3" customWidth="1"/>
     <col min="7" max="7" width="61" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="3"/>
+    <col min="8" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="50" customHeight="1">
+      <c r="A1" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="50" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="50" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="50" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="50" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="50" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="50" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="50" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="D8" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="50" customHeight="1">
+      <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="50" customHeight="1">
+      <c r="A10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="50" customHeight="1">
+      <c r="A11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="1">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="50" customHeight="1">
+      <c r="A12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="50" customHeight="1">
+      <c r="A13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="1">
+        <v>5</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="50" customHeight="1">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="50" customHeight="1">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="B15" s="1">
+        <v>4</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="50" customHeight="1">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
         <v>5</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="C16" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="O1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="3">
-        <v>2</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="3">
-        <v>2</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="3">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="3">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="3">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="3">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B11" s="3">
-        <v>4</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="3">
-        <v>2</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" s="3">
-        <v>5</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="3">
-        <v>2</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="3">
-        <v>4</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="3">
-        <v>5</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="P1" r:id="rId1"/>
-    <hyperlink ref="G11" r:id="rId2"/>
-    <hyperlink ref="J1" r:id="rId3"/>
-    <hyperlink ref="G3" r:id="rId4"/>
+    <hyperlink ref="P1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G11" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="J1" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="82" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="6" max="15" man="1"/>
+  </colBreaks>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1080,12 +1171,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1097,12 +1188,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>